<commit_message>
added week dates and auto highlighting week
</commit_message>
<xml_diff>
--- a/Documents/Draft A/Gantt.xlsx
+++ b/Documents/Draft A/Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B3D33563-EDA0-4DD4-9B84-7467F0BF3D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C635A7F-CB26-4AA4-88F2-19C8B3B275B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Project Planner</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>WEEK (Start 9/8/2024)</t>
+  </si>
+  <si>
+    <t>Winter Break</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -607,6 +610,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -643,8 +649,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1055,10 +1070,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO30"/>
+  <dimension ref="B1:AQ30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="AM3" sqref="AM3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1067,10 +1082,13 @@
     <col min="2" max="2" width="32.33203125" style="2" customWidth="1"/>
     <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
+    <col min="8" max="8" width="3.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16" width="2.77734375" style="1"/>
+    <col min="17" max="27" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="43" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:43" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1078,9 +1096,45 @@
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-    </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="1"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="37"/>
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="37"/>
+    </row>
+    <row r="2" spans="2:43" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="22" t="s">
         <v>29</v>
       </c>
@@ -1092,69 +1146,70 @@
         <v>21</v>
       </c>
       <c r="H2" s="15">
-        <v>10</v>
+        <f ca="1">IF(YEAR(TODAY())=2024, WEEKNUM(TODAY())-36, WEEKNUM(TODAY())+16)</f>
+        <v>7</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="23" t="s">
+      <c r="V2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="34"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="35"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="23" t="s">
+      <c r="AA2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="34"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="35"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="23" t="s">
+      <c r="AI2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AJ2" s="24"/>
-      <c r="AK2" s="24"/>
-      <c r="AL2" s="24"/>
-      <c r="AM2" s="24"/>
-      <c r="AN2" s="24"/>
-      <c r="AO2" s="24"/>
-      <c r="AP2" s="24"/>
-    </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+    </row>
+    <row r="3" spans="2:43" s="12" customFormat="1" ht="39.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="30" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1173,202 +1228,168 @@
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
+      <c r="V3" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+    <row r="4" spans="2:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="3">
+        <f>WEEKNUM(DATE(2024,9,8))-36</f>
         <v>1</v>
       </c>
       <c r="I4" s="3">
+        <f>WEEKNUM(DATE(2024,9,15))-36</f>
         <v>2</v>
       </c>
       <c r="J4" s="3">
+        <f>WEEKNUM(DATE(2024,9,22))-36</f>
         <v>3</v>
       </c>
       <c r="K4" s="3">
+        <f>WEEKNUM(DATE(2024,9,29))-36</f>
         <v>4</v>
       </c>
       <c r="L4" s="3">
+        <f>WEEKNUM(DATE(2024,10,6))-36</f>
         <v>5</v>
       </c>
       <c r="M4" s="3">
+        <f>WEEKNUM(DATE(2024,10,13))-36</f>
         <v>6</v>
       </c>
       <c r="N4" s="3">
+        <f>WEEKNUM(DATE(2024,10,20))-36</f>
         <v>7</v>
       </c>
       <c r="O4" s="3">
+        <f>WEEKNUM(DATE(2024,10,27))-36</f>
         <v>8</v>
       </c>
       <c r="P4" s="3">
+        <f>WEEKNUM(DATE(2024,11,3))-36</f>
         <v>9</v>
       </c>
       <c r="Q4" s="3">
+        <f>WEEKNUM(DATE(2024,11,10))-36</f>
         <v>10</v>
       </c>
       <c r="R4" s="3">
+        <f>WEEKNUM(DATE(2024,11,17))-36</f>
         <v>11</v>
       </c>
       <c r="S4" s="3">
+        <f>WEEKNUM(DATE(2024,11,24))-36</f>
         <v>12</v>
       </c>
       <c r="T4" s="3">
+        <f>WEEKNUM(DATE(2024,12,1))-36</f>
         <v>13</v>
       </c>
       <c r="U4" s="3">
+        <f>WEEKNUM(DATE(2024,12,8))-36</f>
         <v>14</v>
       </c>
       <c r="V4" s="3">
+        <f>WEEKNUM(DATE(2024,12,15))-36</f>
         <v>15</v>
       </c>
       <c r="W4" s="3">
+        <f>WEEKNUM(DATE(2024,12,22))-36</f>
         <v>16</v>
       </c>
       <c r="X4" s="3">
+        <f>WEEKNUM(DATE(2024,12,29))-36</f>
         <v>17</v>
       </c>
       <c r="Y4" s="3">
+        <f>WEEKNUM(DATE(2025,1,5))+16</f>
         <v>18</v>
       </c>
       <c r="Z4" s="3">
+        <f>WEEKNUM(DATE(2025,1,12))+16</f>
         <v>19</v>
       </c>
       <c r="AA4" s="3">
+        <f>WEEKNUM(DATE(2025,1,19))+16</f>
         <v>20</v>
       </c>
       <c r="AB4" s="3">
+        <f>WEEKNUM(DATE(2025,1,26))+16</f>
         <v>21</v>
       </c>
       <c r="AC4" s="3">
+        <f>WEEKNUM(DATE(2025,2,2))+16</f>
         <v>22</v>
       </c>
       <c r="AD4" s="3">
+        <f>WEEKNUM(DATE(2025,2,9))+16</f>
         <v>23</v>
       </c>
       <c r="AE4" s="3">
+        <f>WEEKNUM(DATE(2025,2,16))+16</f>
         <v>24</v>
       </c>
       <c r="AF4" s="3">
+        <f>WEEKNUM(DATE(2025,2,23))+16</f>
         <v>25</v>
       </c>
       <c r="AG4" s="3">
+        <f>WEEKNUM(DATE(2025,3,2))+16</f>
         <v>26</v>
       </c>
       <c r="AH4" s="3">
+        <f>WEEKNUM(DATE(2025,3,9))+16</f>
         <v>27</v>
       </c>
       <c r="AI4" s="3">
+        <f>WEEKNUM(DATE(2025,3,16))+16</f>
         <v>28</v>
       </c>
       <c r="AJ4" s="3">
+        <f>WEEKNUM(DATE(2025,3,23))+16</f>
         <v>29</v>
       </c>
       <c r="AK4" s="3">
+        <f>WEEKNUM(DATE(2025,3,30))+16</f>
         <v>30</v>
       </c>
       <c r="AL4" s="3">
+        <f>WEEKNUM(DATE(2025,4,6))+16</f>
         <v>31</v>
       </c>
       <c r="AM4" s="3">
+        <f>WEEKNUM(DATE(2025,4,13))+16</f>
         <v>32</v>
       </c>
       <c r="AN4" s="3">
+        <f>WEEKNUM(DATE(2025,4,20))+16</f>
         <v>33</v>
       </c>
       <c r="AO4" s="3">
+        <f>WEEKNUM(DATE(2025,4,27))+16</f>
         <v>34</v>
       </c>
       <c r="AP4" s="3">
+        <f>WEEKNUM(DATE(2025,5,4))+16</f>
         <v>35</v>
       </c>
       <c r="AQ4" s="3">
+        <f>WEEKNUM(DATE(2025,5,11))+16</f>
         <v>36</v>
       </c>
-      <c r="AR4" s="3">
-        <v>37</v>
-      </c>
-      <c r="AS4" s="3">
-        <v>38</v>
-      </c>
-      <c r="AT4" s="3">
-        <v>39</v>
-      </c>
-      <c r="AU4" s="3">
-        <v>40</v>
-      </c>
-      <c r="AV4" s="3">
-        <v>41</v>
-      </c>
-      <c r="AW4" s="3">
-        <v>42</v>
-      </c>
-      <c r="AX4" s="3">
-        <v>43</v>
-      </c>
-      <c r="AY4" s="3">
-        <v>44</v>
-      </c>
-      <c r="AZ4" s="3">
-        <v>45</v>
-      </c>
-      <c r="BA4" s="3">
-        <v>46</v>
-      </c>
-      <c r="BB4" s="3">
-        <v>47</v>
-      </c>
-      <c r="BC4" s="3">
-        <v>48</v>
-      </c>
-      <c r="BD4" s="3">
-        <v>49</v>
-      </c>
-      <c r="BE4" s="3">
-        <v>50</v>
-      </c>
-      <c r="BF4" s="3">
-        <v>51</v>
-      </c>
-      <c r="BG4" s="3">
-        <v>52</v>
-      </c>
-      <c r="BH4" s="3">
-        <v>53</v>
-      </c>
-      <c r="BI4" s="3">
-        <v>54</v>
-      </c>
-      <c r="BJ4" s="3">
-        <v>55</v>
-      </c>
-      <c r="BK4" s="3">
-        <v>56</v>
-      </c>
-      <c r="BL4" s="3">
-        <v>57</v>
-      </c>
-      <c r="BM4" s="3">
-        <v>58</v>
-      </c>
-      <c r="BN4" s="3">
-        <v>59</v>
-      </c>
-      <c r="BO4" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
@@ -1388,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
@@ -1408,8 +1429,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="35" t="s">
+    <row r="7" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="7">
@@ -1428,8 +1449,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="35" t="s">
+    <row r="8" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="7">
@@ -1448,8 +1469,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="35" t="s">
+    <row r="9" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="23" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="7">
@@ -1468,8 +1489,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="35" t="s">
+    <row r="10" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="23" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="7">
@@ -1488,8 +1509,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="35" t="s">
+    <row r="11" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="23" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="7">
@@ -1508,8 +1529,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="35" t="s">
+    <row r="12" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="23" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="7">
@@ -1528,8 +1549,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="35" t="s">
+    <row r="13" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="23" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="7">
@@ -1548,8 +1569,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="35" t="s">
+    <row r="14" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="23" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="7">
@@ -1568,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
         <v>2</v>
       </c>
@@ -1588,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
         <v>3</v>
       </c>
@@ -1889,7 +1910,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="AI2:AP2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
@@ -1901,18 +1922,19 @@
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="V3:Z3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B31:BO31">
+  <conditionalFormatting sqref="B31:AQ31">
     <cfRule type="expression" dxfId="9" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:BO4">
+  <conditionalFormatting sqref="H4:AQ4">
     <cfRule type="expression" dxfId="8" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BO30">
+  <conditionalFormatting sqref="H5:AQ30">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>